<commit_message>
Properly implemented ping, implemented setting player properties and coordinates
</commit_message>
<xml_diff>
--- a/Docs/Command map.xlsx
+++ b/Docs/Command map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jochem\Repositories\Prive\GamemakerMultiplayer\GamemakerMultiplayerServer\GamemakerMultiplayerServer\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EF6072-224A-4FE9-86F4-6AEB49705122}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2AA149-66FE-4EB7-B283-DDE3CED7E1B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C552817C-4C83-48CE-87C6-E0123398ECDD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Disconnect</t>
   </si>
@@ -69,10 +69,28 @@
     <t>Properties</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>X, Y, Z, Direction</t>
+    <t>X, Y, Z</t>
+  </si>
+  <si>
+    <t>SPDA</t>
+  </si>
+  <si>
+    <t>SPPO</t>
+  </si>
+  <si>
+    <t>PING</t>
+  </si>
+  <si>
+    <t>Pong's the client.</t>
+  </si>
+  <si>
+    <t>Name, Color, Team</t>
+  </si>
+  <si>
+    <t>Moves the player to a new position</t>
+  </si>
+  <si>
+    <t>Sets the player's properties</t>
   </si>
 </sst>
 </file>
@@ -469,7 +487,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,8 +495,8 @@
     <col min="1" max="1" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
     <col min="3" max="3" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
@@ -516,38 +534,50 @@
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="8"/>
-      <c r="E3" s="6"/>
+      <c r="E3" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="6"/>
+        <v>16</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="6"/>
+        <v>11</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>